<commit_message>
UI design for the question window, and feed back done
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\Desktop\1.MAIN_NEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0284A79F-C09D-4B75-9E8E-2C952957BEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9575ED-7FD8-4DF7-9AF2-3B01C253E9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3756" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>A</t>
   </si>
@@ -37,6 +37,27 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>What are the three buses in a Von Neumann CPU?</t>
+  </si>
+  <si>
+    <t>Data, Memory, Control</t>
+  </si>
+  <si>
+    <t>Control, Register, Memory</t>
+  </si>
+  <si>
+    <t>Data,  Address,  Control</t>
+  </si>
+  <si>
+    <t>Fetch, Decode, Execute</t>
+  </si>
+  <si>
+    <t>The data bus retrieves data and instructions from main memory. The address bus sends addresses to main memory. The control bus sends read right signals to main memory</t>
   </si>
 </sst>
 </file>
@@ -354,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -365,42 +386,45 @@
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
       </c>
       <c r="G1">
         <v>0</v>
       </c>
       <c r="H1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I1">
         <v>1</v>
       </c>
       <c r="J1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K1">
         <v>2</v>
       </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -416,26 +440,29 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>4</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>2</v>
       </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -451,26 +478,29 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="F3" t="s">
+        <v>4</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -486,22 +516,25 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="F4" t="s">
+        <v>4</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testing json question format
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh\Desktop\1.MAIN_NEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9575ED-7FD8-4DF7-9AF2-3B01C253E9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DC8296-8A1F-4E30-9717-E1212EDB0F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3756" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,49 +25,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>feedback</t>
-  </si>
-  <si>
-    <t>What are the three buses in a Von Neumann CPU?</t>
-  </si>
-  <si>
-    <t>Data, Memory, Control</t>
-  </si>
-  <si>
-    <t>Control, Register, Memory</t>
-  </si>
-  <si>
-    <t>Data,  Address,  Control</t>
-  </si>
-  <si>
-    <t>Fetch, Decode, Execute</t>
-  </si>
-  <si>
-    <t>The data bus retrieves data and instructions from main memory. The address bus sends addresses to main memory. The control bus sends read right signals to main memory</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Retrieval</t>
+  </si>
+  <si>
+    <t>What is the purpose of the Accumulator?</t>
+  </si>
+  <si>
+    <t>Holds the result of calculations and operations performed by the arithmetic and logic unit.</t>
+  </si>
+  <si>
+    <t>Holds the data that has been retrieved from memory, or that is about to be stored in memory.</t>
+  </si>
+  <si>
+    <t>Holds the address of the location in memory where data is to be retrieved or stored.</t>
+  </si>
+  <si>
+    <t>Holds the memory location address of the next instruction to be performed by the central processing unit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data bus retrieves data and instructions from main memory. The address bus sends addresses to main memory. The control bus sends read right signals to main memory. </t>
+  </si>
+  <si>
+    <t>The program counter holds the memory location address of the next instruction to be performed by the central processing unit.  Memory data register holds the data that has been retrieved from memory, or that is about to be stored in memory. Accumulator holds the result of calculations and operations performed by the arithmetic and logic unit.</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>Which of the following are examples of Boolaen opeartors</t>
+  </si>
+  <si>
+    <t>The basic boolean operators required for this specification are: OR, NOT, AND, XOR</t>
+  </si>
+  <si>
+    <t>Which of the following can be adjusted to improve the performance of a CPU?</t>
+  </si>
+  <si>
+    <t>Decrease the Cache</t>
+  </si>
+  <si>
+    <t>Remove the OS</t>
+  </si>
+  <si>
+    <t>Get a bigger motherboard</t>
+  </si>
+  <si>
+    <t>Which bus retrieves instructions and data from main memory?</t>
+  </si>
+  <si>
+    <t>Increase the number of cores</t>
+  </si>
+  <si>
+    <t>Each core of a CPU can execute its own independent Fetch Decode Execute (FDE) cycle. A computer with multiple cores can complete more than one FDE cycle at any given time. However to fully utilise multiple cores, the program has be designed in a way that can adapt to this efficiently.</t>
+  </si>
+  <si>
+    <t>WHERE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,7 +425,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,24 +434,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
+      <c r="A1" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1">
         <v>0</v>
       </c>
@@ -412,36 +459,36 @@
         <v>0</v>
       </c>
       <c r="I1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -450,36 +497,36 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3</v>
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -488,36 +535,36 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -526,20 +573,21 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>